<commit_message>
initial commit. Didn't use times yet - just waypoints
</commit_message>
<xml_diff>
--- a/data/inputs_raw/hab_con_ef_time.xlsx
+++ b/data/inputs_raw/hab_con_ef_time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2019-023_Bulkley_fish_passage\scripts\fish_passage_bulkley_2020_reporting\data\inputs_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8682F54-F0C9-41F8-A11C-2F652298F6C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE64FE3E-6C1E-4381-94C4-650700A468CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{F996C734-8ED4-4917-A449-A9115A298CC4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{F996C734-8ED4-4917-A449-A9115A298CC4}"/>
   </bookViews>
   <sheets>
     <sheet name="xref_times" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="103">
   <si>
     <t>site</t>
   </si>
@@ -296,28 +296,55 @@
     <t>197360_us</t>
   </si>
   <si>
-    <t>58159_ds_ef</t>
-  </si>
-  <si>
-    <t>58159_us_ef</t>
-  </si>
-  <si>
-    <t>195290_ds_ef</t>
-  </si>
-  <si>
-    <t>195290_us_ef</t>
-  </si>
-  <si>
-    <t>197360_ds_ef</t>
-  </si>
-  <si>
-    <t>197360_us_ef</t>
-  </si>
-  <si>
     <t>local_name</t>
   </si>
   <si>
     <t>stream_name</t>
+  </si>
+  <si>
+    <t>58159_ds_ef1</t>
+  </si>
+  <si>
+    <t>58159_ds_ef3</t>
+  </si>
+  <si>
+    <t>58159_ds_ef4</t>
+  </si>
+  <si>
+    <t>58159_us_ef1</t>
+  </si>
+  <si>
+    <t>58159_us_ef2</t>
+  </si>
+  <si>
+    <t>58159_us_ef3</t>
+  </si>
+  <si>
+    <t>58159_us_ef4</t>
+  </si>
+  <si>
+    <t>195290_us_ef1</t>
+  </si>
+  <si>
+    <t>195290_ds_ef1</t>
+  </si>
+  <si>
+    <t>195290_us_ef2</t>
+  </si>
+  <si>
+    <t>197663_ds_ef1</t>
+  </si>
+  <si>
+    <t>197663_us_ef1</t>
+  </si>
+  <si>
+    <t>197360_us_ef1</t>
+  </si>
+  <si>
+    <t>197360_us_ef2</t>
+  </si>
+  <si>
+    <t>197360_ds_ef1</t>
   </si>
 </sst>
 </file>
@@ -1226,23 +1253,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B96CC020-EA98-438A-98FF-317968827C67}">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C1" t="s">
         <v>28</v>
@@ -1708,7 +1736,19 @@
         <v>76</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>88</v>
+      </c>
+      <c r="C42">
+        <v>68</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>627533</v>
+      </c>
+      <c r="F42">
+        <v>6060447</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1716,42 +1756,267 @@
         <v>76</v>
       </c>
       <c r="B43" t="s">
-        <v>87</v>
+        <v>27</v>
+      </c>
+      <c r="C43">
+        <v>69</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>627555</v>
+      </c>
+      <c r="F43">
+        <v>6060461</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B44" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+      <c r="C44">
+        <v>71</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>627585</v>
+      </c>
+      <c r="F44">
+        <v>6060475</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B45" t="s">
-        <v>89</v>
+        <v>90</v>
+      </c>
+      <c r="C45">
+        <v>72</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>627611</v>
+      </c>
+      <c r="F45">
+        <v>6060455</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B46" t="s">
-        <v>90</v>
+        <v>91</v>
+      </c>
+      <c r="C46">
+        <v>74</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>627669</v>
+      </c>
+      <c r="F46">
+        <v>6060433</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" t="s">
+        <v>92</v>
+      </c>
+      <c r="C47">
+        <v>75</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>627702</v>
+      </c>
+      <c r="F47">
+        <v>6060433</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>76</v>
+      </c>
+      <c r="B48" t="s">
+        <v>93</v>
+      </c>
+      <c r="E48">
+        <v>627793</v>
+      </c>
+      <c r="F48">
+        <v>6060395</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" t="s">
+        <v>94</v>
+      </c>
+      <c r="E49">
+        <v>628003</v>
+      </c>
+      <c r="F49">
+        <v>6060508</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50" t="s">
+        <v>95</v>
+      </c>
+      <c r="E50">
+        <v>640028</v>
+      </c>
+      <c r="F50">
+        <v>6051717</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>79</v>
+      </c>
+      <c r="B51" t="s">
+        <v>96</v>
+      </c>
+      <c r="E51">
+        <v>639984</v>
+      </c>
+      <c r="F51">
+        <v>6051683</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>79</v>
+      </c>
+      <c r="B52" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52">
+        <v>97</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>640890</v>
+      </c>
+      <c r="F52">
+        <v>6051588</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>71</v>
+      </c>
+      <c r="B53" t="s">
+        <v>98</v>
+      </c>
+      <c r="C53">
+        <v>66</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>670225</v>
+      </c>
+      <c r="F53">
+        <v>6044638</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>71</v>
+      </c>
+      <c r="B54" t="s">
+        <v>99</v>
+      </c>
+      <c r="C54">
+        <v>53</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>670225</v>
+      </c>
+      <c r="F54">
+        <v>6044812</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>83</v>
       </c>
-      <c r="B47" t="s">
-        <v>91</v>
+      <c r="B55" t="s">
+        <v>100</v>
+      </c>
+      <c r="C55">
+        <v>268</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="E55">
+        <v>650101</v>
+      </c>
+      <c r="F55">
+        <v>5992660</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>83</v>
+      </c>
+      <c r="B56" t="s">
+        <v>101</v>
+      </c>
+      <c r="E56">
+        <v>650179</v>
+      </c>
+      <c r="F56">
+        <v>5992702</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>83</v>
+      </c>
+      <c r="B57" t="s">
+        <v>102</v>
+      </c>
+      <c r="E57">
+        <v>649896</v>
+      </c>
+      <c r="F57">
+        <v>5992406</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>